<commit_message>
Hoàn thành kết nối ngoại vi 25/03
</commit_message>
<xml_diff>
--- a/PINOUT_STM32.xlsx
+++ b/PINOUT_STM32.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>PORT</t>
   </si>
@@ -34,13 +34,130 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>ENCA_RIGHT</t>
+  </si>
+  <si>
+    <t>ENCB_RIGHT</t>
+  </si>
+  <si>
+    <t>SENSOR_1</t>
+  </si>
+  <si>
+    <t>SENSOR_2</t>
+  </si>
+  <si>
+    <t>PWM_LIFT</t>
+  </si>
+  <si>
+    <t>DIR_LIFT</t>
+  </si>
+  <si>
+    <t>PWM_LEFT</t>
+  </si>
+  <si>
+    <t>PWM_RIGHT</t>
+  </si>
+  <si>
+    <t>DIR__LEFT</t>
+  </si>
+  <si>
+    <t>DIR_RIGHT</t>
+  </si>
+  <si>
+    <t>LCD_SDA</t>
+  </si>
+  <si>
+    <t>LCD_SCL</t>
+  </si>
+  <si>
+    <t>ENCA_LIFT</t>
+  </si>
+  <si>
+    <t>ENCB_LIFT</t>
+  </si>
+  <si>
+    <t>RFID_SDA</t>
+  </si>
+  <si>
+    <t>RFID_SCK</t>
+  </si>
+  <si>
+    <t>RFID_MISO</t>
+  </si>
+  <si>
+    <t>RFID_MOSI</t>
+  </si>
+  <si>
+    <t>QTR_IN1</t>
+  </si>
+  <si>
+    <t>QTR_IN2</t>
+  </si>
+  <si>
+    <t>QTR_IN3</t>
+  </si>
+  <si>
+    <t>QTR_IN4</t>
+  </si>
+  <si>
+    <t>QTR_IN5</t>
+  </si>
+  <si>
+    <t>UART_Tx</t>
+  </si>
+  <si>
+    <t>UART_Rx</t>
+  </si>
+  <si>
+    <t>ENCA_LEFT</t>
+  </si>
+  <si>
+    <t>ENCB_LEFT</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>ENCODER</t>
+  </si>
+  <si>
+    <t>QTR-5RC</t>
+  </si>
+  <si>
+    <t>RFID</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>SENSOR</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,8 +165,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,18 +200,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -104,31 +252,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,75 +632,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="9">
         <v>0</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="9">
         <v>1</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="9">
         <v>2</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="9">
         <v>3</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="9">
         <v>4</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="9">
         <v>5</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="9">
         <v>6</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="9">
         <v>7</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="9">
         <v>8</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="9">
         <v>9</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="9">
         <v>10</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="9">
         <v>11</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="9">
         <v>12</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="9">
         <v>13</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="9">
         <v>14</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R1" s="9">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -490,34 +731,54 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="9"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="7"/>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
@@ -526,58 +787,131 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="L4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="6"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>1</v>
+      <c r="B8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>2</v>
+      <c r="B9" s="12"/>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>3</v>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>